<commit_message>
Roles, control duplicados y limpieza de credenciales
</commit_message>
<xml_diff>
--- a/registro_montaje.xlsx
+++ b/registro_montaje.xlsx
@@ -16,11 +16,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
     <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
-    <numFmt numFmtId="166" formatCode="yyyy-mm-dd"/>
-    <numFmt numFmtId="167" formatCode="YYYY-MM-DD"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -60,13 +58,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -432,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:L20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -481,6 +478,26 @@
           <t>Observaciones</t>
         </is>
       </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Nombre</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Hora inicio</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Hora fin</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>CHECK LIST</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -509,6 +526,10 @@
         </is>
       </c>
       <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -541,6 +562,10 @@
           <t>malas condiciones climatologicas</t>
         </is>
       </c>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -573,6 +598,10 @@
           <t>esta bien</t>
         </is>
       </c>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -605,6 +634,10 @@
           <t>kkkkkkkkkkkkkkk</t>
         </is>
       </c>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -633,6 +666,10 @@
         </is>
       </c>
       <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
+      <c r="L6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -661,6 +698,10 @@
         </is>
       </c>
       <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr"/>
+      <c r="L7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -689,6 +730,10 @@
         </is>
       </c>
       <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
+      <c r="L8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -717,6 +762,10 @@
         </is>
       </c>
       <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="inlineStr"/>
+      <c r="K9" t="inlineStr"/>
+      <c r="L9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -745,6 +794,10 @@
         </is>
       </c>
       <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr"/>
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -773,6 +826,10 @@
         </is>
       </c>
       <c r="H11" t="inlineStr"/>
+      <c r="I11" t="inlineStr"/>
+      <c r="J11" t="inlineStr"/>
+      <c r="K11" t="inlineStr"/>
+      <c r="L11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -801,6 +858,10 @@
         </is>
       </c>
       <c r="H12" t="inlineStr"/>
+      <c r="I12" t="inlineStr"/>
+      <c r="J12" t="inlineStr"/>
+      <c r="K12" t="inlineStr"/>
+      <c r="L12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -829,6 +890,10 @@
         </is>
       </c>
       <c r="H13" t="inlineStr"/>
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" t="inlineStr"/>
+      <c r="K13" t="inlineStr"/>
+      <c r="L13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -857,6 +922,10 @@
         </is>
       </c>
       <c r="H14" t="inlineStr"/>
+      <c r="I14" t="inlineStr"/>
+      <c r="J14" t="inlineStr"/>
+      <c r="K14" t="inlineStr"/>
+      <c r="L14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -885,6 +954,10 @@
         </is>
       </c>
       <c r="H15" t="inlineStr"/>
+      <c r="I15" t="inlineStr"/>
+      <c r="J15" t="inlineStr"/>
+      <c r="K15" t="inlineStr"/>
+      <c r="L15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -917,6 +990,10 @@
           <t>es la prueba final</t>
         </is>
       </c>
+      <c r="I16" t="inlineStr"/>
+      <c r="J16" t="inlineStr"/>
+      <c r="K16" t="inlineStr"/>
+      <c r="L16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -945,12 +1022,16 @@
         </is>
       </c>
       <c r="H17" t="inlineStr"/>
+      <c r="I17" t="inlineStr"/>
+      <c r="J17" t="inlineStr"/>
+      <c r="K17" t="inlineStr"/>
+      <c r="L17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="n">
         <v>1</v>
       </c>
-      <c r="B18" s="3" t="n">
+      <c r="B18" s="2" t="n">
         <v>45977</v>
       </c>
       <c r="C18" t="n">
@@ -975,6 +1056,90 @@
       <c r="H18" t="inlineStr">
         <is>
           <t>pruba web</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr"/>
+      <c r="J18" t="inlineStr"/>
+      <c r="K18" t="inlineStr"/>
+      <c r="L18" t="inlineStr"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>1</v>
+      </c>
+      <c r="B19" s="2" t="n">
+        <v>45977</v>
+      </c>
+      <c r="C19" t="n">
+        <v>1</v>
+      </c>
+      <c r="D19" t="n">
+        <v>7</v>
+      </c>
+      <c r="E19" t="n">
+        <v>8</v>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr"/>
+      <c r="I19" t="inlineStr"/>
+      <c r="J19" t="inlineStr"/>
+      <c r="K19" t="inlineStr"/>
+      <c r="L19" t="inlineStr"/>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>31</v>
+      </c>
+      <c r="B20" s="2" t="n">
+        <v>45979</v>
+      </c>
+      <c r="C20" t="n">
+        <v>1</v>
+      </c>
+      <c r="D20" t="n">
+        <v>10</v>
+      </c>
+      <c r="E20" t="n">
+        <v>11</v>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>NO OK</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr"/>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>RUBEN ALVAREZ FERNANDEZ</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>09:56</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>09:57</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>OK</t>
         </is>
       </c>
     </row>

</xml_diff>